<commit_message>
Cahier des charges + Spé détaillées Accueil finit + script sql contrainte & structure
</commit_message>
<xml_diff>
--- a/Base de données/Jeu de données.xlsx
+++ b/Base de données/Jeu de données.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
   <si>
     <t>IdTypeEmploye</t>
   </si>
@@ -438,6 +438,21 @@
   </si>
   <si>
     <t>Chèque Vacances</t>
+  </si>
+  <si>
+    <t>8.99</t>
+  </si>
+  <si>
+    <t>14.99</t>
+  </si>
+  <si>
+    <t>54.99</t>
+  </si>
+  <si>
+    <t>69.99</t>
+  </si>
+  <si>
+    <t>134.99</t>
   </si>
 </sst>
 </file>
@@ -593,7 +608,37 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
@@ -715,12 +760,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C4" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="IdTypeEmploye" dataDxfId="8"/>
-    <tableColumn id="2" name="LibelleTypeEmploye" dataDxfId="7"/>
-    <tableColumn id="3" name="Colonne1" dataDxfId="3">
+    <tableColumn id="1" name="IdTypeEmploye" dataDxfId="18"/>
+    <tableColumn id="2" name="LibelleTypeEmploye" dataDxfId="17"/>
+    <tableColumn id="3" name="Colonne1" dataDxfId="13">
       <calculatedColumnFormula>"INSERT INTO TypeEmploye VALUES (" &amp; Tableau1[[#This Row],[IdTypeEmploye]] &amp; ", """ &amp; Tableau1[[#This Row],[LibelleTypeEmploye]] &amp; """);"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -729,25 +774,31 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="D32:G37" totalsRowShown="0">
-  <autoFilter ref="D32:G37"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="D32:H37" totalsRowShown="0">
+  <autoFilter ref="D32:H37"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="IdPrestation"/>
     <tableColumn id="2" name="LibellePrestation"/>
     <tableColumn id="3" name="DescriptionPrestation"/>
     <tableColumn id="4" name="PrixPrestation"/>
+    <tableColumn id="5" name="Colonne1" dataDxfId="1">
+      <calculatedColumnFormula>"INSERT INTO Prestations VALUES(" &amp; Tableau10[[#This Row],[IdPrestation]] &amp; ",""" &amp; Tableau10[[#This Row],[LibellePrestation]] &amp; """,""" &amp; Tableau10[[#This Row],[DescriptionPrestation]] &amp; """," &amp; Tableau10[[#This Row],[PrixPrestation]] &amp; ");"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A40:C44" totalsRowShown="0">
-  <autoFilter ref="A40:C44"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau11" displayName="Tableau11" ref="A40:D44" totalsRowShown="0">
+  <autoFilter ref="A40:D44"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="IdFidelite"/>
     <tableColumn id="2" name="LibelleFidelite"/>
-    <tableColumn id="3" name="DescriptionFidelite" dataDxfId="5"/>
+    <tableColumn id="3" name="DescriptionFidelite" dataDxfId="15"/>
+    <tableColumn id="4" name="Colonne1" dataDxfId="0">
+      <calculatedColumnFormula>"INSERT INTO Fidelites VALUES(" &amp; Tableau11[[#This Row],[IdFidelite]] &amp; ",""" &amp; Tableau11[[#This Row],[LibelleFidelite]] &amp; """,""" &amp; Tableau11[[#This Row],[DescriptionFidelite]] &amp; """);"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -760,7 +811,7 @@
     <tableColumn id="1" name="IdHistoriqueNettoyage"/>
     <tableColumn id="2" name="Employé"/>
     <tableColumn id="3" name="Chambre"/>
-    <tableColumn id="4" name="DateHeure" dataDxfId="4"/>
+    <tableColumn id="4" name="DateHeure" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -812,8 +863,8 @@
   <tableColumns count="7">
     <tableColumn id="1" name="IdReservation"/>
     <tableColumn id="2" name="NumReservation"/>
-    <tableColumn id="3" name="DateDebut" dataDxfId="2"/>
-    <tableColumn id="4" name="DateFin" dataDxfId="1"/>
+    <tableColumn id="3" name="DateDebut" dataDxfId="12"/>
+    <tableColumn id="4" name="DateFin" dataDxfId="11"/>
     <tableColumn id="5" name="NbPersonnes"/>
     <tableColumn id="6" name="NbChambres"/>
     <tableColumn id="7" name="Client"/>
@@ -829,7 +880,7 @@
     <tableColumn id="1" name="IdHistoriqueActions"/>
     <tableColumn id="2" name="Employe"/>
     <tableColumn id="3" name="Reservation"/>
-    <tableColumn id="4" name="DateHeure" dataDxfId="0"/>
+    <tableColumn id="4" name="DateHeure" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,98 +902,122 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="D1:I6" totalsRowShown="0">
-  <autoFilter ref="D1:I6"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="D1:J6" totalsRowShown="0">
+  <autoFilter ref="D1:J6"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="IdEmploye"/>
     <tableColumn id="2" name="NomEmploye"/>
     <tableColumn id="3" name="PrenomEmploye"/>
     <tableColumn id="4" name="Identifiant"/>
     <tableColumn id="5" name="Mdp"/>
     <tableColumn id="6" name="Rôle"/>
+    <tableColumn id="7" name="Colonne1" dataDxfId="9">
+      <calculatedColumnFormula>"INSERT INTO Employes VALUES(" &amp; Tableau2[[#This Row],[IdEmploye]] &amp; ",""" &amp; Tableau2[[#This Row],[NomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[PrenomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[Identifiant]] &amp; """,""" &amp; Tableau2[[#This Row],[Mdp]] &amp; """," &amp; Tableau2[[#This Row],[Rôle]] &amp; ");"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A9:C14" totalsRowShown="0">
-  <autoFilter ref="A9:C14"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A9:D14" totalsRowShown="0">
+  <autoFilter ref="A9:D14"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="IdTypeChambre"/>
     <tableColumn id="2" name="LibelleTypeChambre"/>
     <tableColumn id="3" name="PrixChambre"/>
+    <tableColumn id="4" name="Colonne1" dataDxfId="8">
+      <calculatedColumnFormula>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; C11 &amp; ");"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="E9:G12" totalsRowShown="0">
-  <autoFilter ref="E9:G12"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="E9:H12" totalsRowShown="0">
+  <autoFilter ref="E9:H12"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="IdEquipementChambre"/>
     <tableColumn id="2" name="LibelleEquipementChambre"/>
     <tableColumn id="3" name="DescriptionEquipementChambre"/>
+    <tableColumn id="4" name="Colonne1" dataDxfId="7">
+      <calculatedColumnFormula>"INSERT INTO EquipementsChambres VALUES(" &amp; Tableau4[[#This Row],[IdEquipementChambre]] &amp; ",""" &amp; Tableau4[[#This Row],[LibelleEquipementChambre]] &amp; """,""" &amp; Tableau4[[#This Row],[DescriptionEquipementChambre]] &amp; """);"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A17:B21" totalsRowShown="0">
-  <autoFilter ref="A17:B21"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A17:C21" totalsRowShown="0">
+  <autoFilter ref="A17:C21"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="IdEtage"/>
     <tableColumn id="2" name="NumEtage"/>
+    <tableColumn id="3" name="Colonne1" dataDxfId="6">
+      <calculatedColumnFormula>"INSERT INTO Etages VALUES(" &amp; Tableau5[[#This Row],[IdEtage]] &amp; "," &amp; Tableau5[[#This Row],[NumEtage]] &amp;");"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="D17:E20" totalsRowShown="0">
-  <autoFilter ref="D17:E20"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="D17:F20" totalsRowShown="0">
+  <autoFilter ref="D17:F20"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="IdStatutChambre"/>
     <tableColumn id="2" name="LibelleStatutChambre"/>
+    <tableColumn id="3" name="Colonne1" dataDxfId="5">
+      <calculatedColumnFormula>"INSERT INTO StatutsChambres VALUES(" &amp; Tableau6[[#This Row],[IdStatutChambre]] &amp; ",""" &amp; Tableau6[[#This Row],[LibelleStatutChambre]] &amp; """);"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="A24:E29" totalsRowShown="0">
-  <autoFilter ref="A24:E29"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="A24:F29" totalsRowShown="0">
+  <autoFilter ref="A24:F29"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="IdChambre"/>
     <tableColumn id="2" name="NumChambre"/>
     <tableColumn id="3" name="TypeChambre"/>
     <tableColumn id="4" name="StatutChambre"/>
     <tableColumn id="5" name="Etage"/>
+    <tableColumn id="6" name="Colonne1" dataDxfId="4">
+      <calculatedColumnFormula>"INSERT INTO Chambres VALUES(" &amp; Tableau7[[#This Row],[IdChambre]] &amp; "," &amp; Tableau7[[#This Row],[NumChambre]] &amp; "," &amp; Tableau7[[#This Row],[TypeChambre]] &amp; "," &amp; Tableau7[[#This Row],[StatutChambre]] &amp; "," &amp; Tableau7[[#This Row],[Etage]] &amp; ");"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="G24:I29" totalsRowShown="0">
-  <autoFilter ref="G24:I29"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="G24:J29" totalsRowShown="0">
+  <autoFilter ref="G24:J29"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="IdPossessionEquipement"/>
     <tableColumn id="2" name="Chambre"/>
     <tableColumn id="3" name="Equipement"/>
+    <tableColumn id="4" name="Colonne1" dataDxfId="3">
+      <calculatedColumnFormula>"INSERT INTO PossessionsEquipements VALUES(" &amp; Tableau8[[#This Row],[IdPossessionEquipement]] &amp; "," &amp; Tableau8[[#This Row],[Chambre]] &amp;"," &amp; Tableau8[[#This Row],[Equipement]] &amp;");"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A32:B36" totalsRowShown="0">
-  <autoFilter ref="A32:B36"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A32:C36" totalsRowShown="0">
+  <autoFilter ref="A32:C36"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="IdTypePaiement"/>
     <tableColumn id="2" name="LibelleTypePaiement"/>
+    <tableColumn id="3" name="Colonne1" dataDxfId="2">
+      <calculatedColumnFormula>"INSERT INTO TypesPaiements VALUES(" &amp; Tableau9[[#This Row],[IdTypePaiement]] &amp; ",""" &amp; Tableau9[[#This Row],[LibelleTypePaiement]] &amp; """);"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1211,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,13 +1299,14 @@
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" customWidth="1"/>
     <col min="7" max="7" width="57" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="125.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1258,8 +1334,11 @@
       <c r="I1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1285,11 +1364,15 @@
       <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
+        <f>"INSERT INTO Employes VALUES(" &amp; Tableau2[[#This Row],[IdEmploye]] &amp; ",""" &amp; Tableau2[[#This Row],[NomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[PrenomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[Identifiant]] &amp; """,""" &amp; Tableau2[[#This Row],[Mdp]] &amp; """," &amp; Tableau2[[#This Row],[Rôle]] &amp; ");"</f>
+        <v>INSERT INTO Employes VALUES(1,"Dupond","Jean","j.dupond","jbvmzr145Gqlkdjfghqmehbmdjbhmzkeghlmzqejbhbhtr",1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1315,11 +1398,15 @@
       <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="str">
+        <f>"INSERT INTO Employes VALUES(" &amp; Tableau2[[#This Row],[IdEmploye]] &amp; ",""" &amp; Tableau2[[#This Row],[NomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[PrenomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[Identifiant]] &amp; """,""" &amp; Tableau2[[#This Row],[Mdp]] &amp; """," &amp; Tableau2[[#This Row],[Rôle]] &amp; ");"</f>
+        <v>INSERT INTO Employes VALUES(2,"Avotservice","Gilbert","g.avotservice","jszhdikuzjsehrgmozerbgmozejrbgmkezbmoeeRG4",2);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1345,11 +1432,15 @@
       <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"INSERT INTO Employes VALUES(" &amp; Tableau2[[#This Row],[IdEmploye]] &amp; ",""" &amp; Tableau2[[#This Row],[NomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[PrenomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[Identifiant]] &amp; """,""" &amp; Tableau2[[#This Row],[Mdp]] &amp; """," &amp; Tableau2[[#This Row],[Rôle]] &amp; ");"</f>
+        <v>INSERT INTO Employes VALUES(3,"Uitout","Jess","j.uitout","kfbkfnbir!5uhgmieqzrjbgmizearbglmizerqbiblrez",3);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>4</v>
       </c>
@@ -1365,11 +1456,15 @@
       <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="str">
+        <f>"INSERT INTO Employes VALUES(" &amp; Tableau2[[#This Row],[IdEmploye]] &amp; ",""" &amp; Tableau2[[#This Row],[NomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[PrenomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[Identifiant]] &amp; """,""" &amp; Tableau2[[#This Row],[Mdp]] &amp; """," &amp; Tableau2[[#This Row],[Rôle]] &amp; ");"</f>
+        <v>INSERT INTO Employes VALUES(4,"Duchmol","Pierre","p.duchmol","fgjbkljfgdh21smrgzheùoihgzmeorhgmzlerngmze",2);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>5</v>
       </c>
@@ -1385,11 +1480,15 @@
       <c r="H6" t="s">
         <v>30</v>
       </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="str">
+        <f>"INSERT INTO Employes VALUES(" &amp; Tableau2[[#This Row],[IdEmploye]] &amp; ",""" &amp; Tableau2[[#This Row],[NomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[PrenomEmploye]] &amp; """,""" &amp; Tableau2[[#This Row],[Identifiant]] &amp; """,""" &amp; Tableau2[[#This Row],[Mdp]] &amp; """," &amp; Tableau2[[#This Row],[Rôle]] &amp; ");"</f>
+        <v>INSERT INTO Employes VALUES(5,"Patate","Micheline","m.patate","AQEThetha!581qdf14dfg65er4g6e4g65er4ge65rghetrqaethzetheryj",3);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1399,6 +1498,9 @@
       <c r="C9" t="s">
         <v>40</v>
       </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
       <c r="E9" t="s">
         <v>46</v>
       </c>
@@ -1408,8 +1510,11 @@
       <c r="G9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1419,6 +1524,10 @@
       <c r="C10">
         <v>50</v>
       </c>
+      <c r="D10" t="str">
+        <f>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; C11 &amp; ");"</f>
+        <v>INSERT INTO TypesChambres VALUES(1,"Standard Simple",54.99);</v>
+      </c>
       <c r="E10">
         <v>1</v>
       </c>
@@ -1428,16 +1537,24 @@
       <c r="G10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f>"INSERT INTO EquipementsChambres VALUES(" &amp; Tableau4[[#This Row],[IdEquipementChambre]] &amp; ",""" &amp; Tableau4[[#This Row],[LibelleEquipementChambre]] &amp; """,""" &amp; Tableau4[[#This Row],[DescriptionEquipementChambre]] &amp; """);"</f>
+        <v>INSERT INTO EquipementsChambres VALUES(1,"Coffre-fort","Un coffre-fort pour stocker les objets de valeurs en sécurité");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11">
-        <v>54.99</v>
+      <c r="C11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" t="str">
+        <f>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; C12 &amp; ");"</f>
+        <v>INSERT INTO TypesChambres VALUES(2,"Standard Double",65);</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1448,8 +1565,12 @@
       <c r="G11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f>"INSERT INTO EquipementsChambres VALUES(" &amp; Tableau4[[#This Row],[IdEquipementChambre]] &amp; ",""" &amp; Tableau4[[#This Row],[LibelleEquipementChambre]] &amp; """,""" &amp; Tableau4[[#This Row],[DescriptionEquipementChambre]] &amp; """);"</f>
+        <v>INSERT INTO EquipementsChambres VALUES(2,"Mini-bar","Un mini-bar rempli de différentes boissons alcoolisées ou non");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1459,6 +1580,10 @@
       <c r="C12">
         <v>65</v>
       </c>
+      <c r="D12" t="str">
+        <f>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; C13 &amp; ");"</f>
+        <v>INSERT INTO TypesChambres VALUES(3,"Deluxe Simple",69.99);</v>
+      </c>
       <c r="E12">
         <v>3</v>
       </c>
@@ -1468,63 +1593,93 @@
       <c r="G12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f>"INSERT INTO EquipementsChambres VALUES(" &amp; Tableau4[[#This Row],[IdEquipementChambre]] &amp; ",""" &amp; Tableau4[[#This Row],[LibelleEquipementChambre]] &amp; """,""" &amp; Tableau4[[#This Row],[DescriptionEquipementChambre]] &amp; """);"</f>
+        <v>INSERT INTO EquipementsChambres VALUES(3,"Climatisation","Une climatisation pour réguler la température de la chambre");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="C13">
-        <v>69.989999999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" t="str">
+        <f>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; C14 &amp; ");"</f>
+        <v>INSERT INTO TypesChambres VALUES(4,"Deluxe Double",134.99);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C14">
-        <v>134.99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" t="str">
+        <f>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; C15 &amp; ");"</f>
+        <v>INSERT INTO TypesChambres VALUES(5,"Suite",);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
       </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
       <c r="D17" t="s">
         <v>57</v>
       </c>
       <c r="E17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
+      <c r="C18" t="str">
+        <f>"INSERT INTO Etages VALUES(" &amp; Tableau5[[#This Row],[IdEtage]] &amp; "," &amp; Tableau5[[#This Row],[NumEtage]] &amp;");"</f>
+        <v>INSERT INTO Etages VALUES(1,0);</v>
+      </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f>"INSERT INTO StatutsChambres VALUES(" &amp; Tableau6[[#This Row],[IdStatutChambre]] &amp; ",""" &amp; Tableau6[[#This Row],[LibelleStatutChambre]] &amp; """);"</f>
+        <v>INSERT INTO StatutsChambres VALUES(1,"Libre");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19">
         <v>1</v>
+      </c>
+      <c r="C19" t="str">
+        <f>"INSERT INTO Etages VALUES(" &amp; Tableau5[[#This Row],[IdEtage]] &amp; "," &amp; Tableau5[[#This Row],[NumEtage]] &amp;");"</f>
+        <v>INSERT INTO Etages VALUES(2,1);</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1532,13 +1687,21 @@
       <c r="E19" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f>"INSERT INTO StatutsChambres VALUES(" &amp; Tableau6[[#This Row],[IdStatutChambre]] &amp; ",""" &amp; Tableau6[[#This Row],[LibelleStatutChambre]] &amp; """);"</f>
+        <v>INSERT INTO StatutsChambres VALUES(2,"Occupé");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20">
         <v>2</v>
+      </c>
+      <c r="C20" t="str">
+        <f>"INSERT INTO Etages VALUES(" &amp; Tableau5[[#This Row],[IdEtage]] &amp; "," &amp; Tableau5[[#This Row],[NumEtage]] &amp;");"</f>
+        <v>INSERT INTO Etages VALUES(3,2);</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1546,16 +1709,24 @@
       <c r="E20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f>"INSERT INTO StatutsChambres VALUES(" &amp; Tableau6[[#This Row],[IdStatutChambre]] &amp; ",""" &amp; Tableau6[[#This Row],[LibelleStatutChambre]] &amp; """);"</f>
+        <v>INSERT INTO StatutsChambres VALUES(3,"Nettoyage en cours");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="str">
+        <f>"INSERT INTO Etages VALUES(" &amp; Tableau5[[#This Row],[IdEtage]] &amp; "," &amp; Tableau5[[#This Row],[NumEtage]] &amp;");"</f>
+        <v>INSERT INTO Etages VALUES(4,3);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1571,6 +1742,9 @@
       <c r="E24" t="s">
         <v>66</v>
       </c>
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
       <c r="G24" t="s">
         <v>67</v>
       </c>
@@ -1580,144 +1754,190 @@
       <c r="I24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25">
         <v>101</v>
       </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F25" t="str">
+        <f>"INSERT INTO Chambres VALUES(" &amp; Tableau7[[#This Row],[IdChambre]] &amp; "," &amp; Tableau7[[#This Row],[NumChambre]] &amp; "," &amp; Tableau7[[#This Row],[TypeChambre]] &amp; "," &amp; Tableau7[[#This Row],[StatutChambre]] &amp; "," &amp; Tableau7[[#This Row],[Etage]] &amp; ");"</f>
+        <v>INSERT INTO Chambres VALUES(1,101,1,1,2);</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>201</v>
-      </c>
-      <c r="I25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="str">
+        <f>"INSERT INTO PossessionsEquipements VALUES(" &amp; Tableau8[[#This Row],[IdPossessionEquipement]] &amp; "," &amp; Tableau8[[#This Row],[Chambre]] &amp;"," &amp; Tableau8[[#This Row],[Equipement]] &amp;");"</f>
+        <v>INSERT INTO PossessionsEquipements VALUES(1,3,1);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26">
         <v>102</v>
       </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F26" t="str">
+        <f>"INSERT INTO Chambres VALUES(" &amp; Tableau7[[#This Row],[IdChambre]] &amp; "," &amp; Tableau7[[#This Row],[NumChambre]] &amp; "," &amp; Tableau7[[#This Row],[TypeChambre]] &amp; "," &amp; Tableau7[[#This Row],[StatutChambre]] &amp; "," &amp; Tableau7[[#This Row],[Etage]] &amp; ");"</f>
+        <v>INSERT INTO Chambres VALUES(2,102,1,2,2);</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="H26">
-        <v>202</v>
-      </c>
-      <c r="I26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="str">
+        <f>"INSERT INTO PossessionsEquipements VALUES(" &amp; Tableau8[[#This Row],[IdPossessionEquipement]] &amp; "," &amp; Tableau8[[#This Row],[Chambre]] &amp;"," &amp; Tableau8[[#This Row],[Equipement]] &amp;");"</f>
+        <v>INSERT INTO PossessionsEquipements VALUES(2,4,1);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
       <c r="B27">
         <v>201</v>
       </c>
-      <c r="C27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F27" t="str">
+        <f>"INSERT INTO Chambres VALUES(" &amp; Tableau7[[#This Row],[IdChambre]] &amp; "," &amp; Tableau7[[#This Row],[NumChambre]] &amp; "," &amp; Tableau7[[#This Row],[TypeChambre]] &amp; "," &amp; Tableau7[[#This Row],[StatutChambre]] &amp; "," &amp; Tableau7[[#This Row],[Etage]] &amp; ");"</f>
+        <v>INSERT INTO Chambres VALUES(3,201,3,3,3);</v>
       </c>
       <c r="G27">
         <v>3</v>
       </c>
       <c r="H27">
-        <v>301</v>
-      </c>
-      <c r="I27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="str">
+        <f>"INSERT INTO PossessionsEquipements VALUES(" &amp; Tableau8[[#This Row],[IdPossessionEquipement]] &amp; "," &amp; Tableau8[[#This Row],[Chambre]] &amp;"," &amp; Tableau8[[#This Row],[Equipement]] &amp;");"</f>
+        <v>INSERT INTO PossessionsEquipements VALUES(3,5,1);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
       <c r="B28">
         <v>202</v>
       </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>59</v>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F28" t="str">
+        <f>"INSERT INTO Chambres VALUES(" &amp; Tableau7[[#This Row],[IdChambre]] &amp; "," &amp; Tableau7[[#This Row],[NumChambre]] &amp; "," &amp; Tableau7[[#This Row],[TypeChambre]] &amp; "," &amp; Tableau7[[#This Row],[StatutChambre]] &amp; "," &amp; Tableau7[[#This Row],[Etage]] &amp; ");"</f>
+        <v>INSERT INTO Chambres VALUES(4,202,3,1,3);</v>
       </c>
       <c r="G28">
         <v>4</v>
       </c>
       <c r="H28">
-        <v>301</v>
-      </c>
-      <c r="I28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28" t="str">
+        <f>"INSERT INTO PossessionsEquipements VALUES(" &amp; Tableau8[[#This Row],[IdPossessionEquipement]] &amp; "," &amp; Tableau8[[#This Row],[Chambre]] &amp;"," &amp; Tableau8[[#This Row],[Equipement]] &amp;");"</f>
+        <v>INSERT INTO PossessionsEquipements VALUES(4,5,2);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29">
         <v>301</v>
       </c>
-      <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" t="s">
-        <v>60</v>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="F29" t="str">
+        <f>"INSERT INTO Chambres VALUES(" &amp; Tableau7[[#This Row],[IdChambre]] &amp; "," &amp; Tableau7[[#This Row],[NumChambre]] &amp; "," &amp; Tableau7[[#This Row],[TypeChambre]] &amp; "," &amp; Tableau7[[#This Row],[StatutChambre]] &amp; "," &amp; Tableau7[[#This Row],[Etage]] &amp; ");"</f>
+        <v>INSERT INTO Chambres VALUES(5,301,5,2,4);</v>
       </c>
       <c r="G29">
         <v>5</v>
       </c>
       <c r="H29">
-        <v>301</v>
-      </c>
-      <c r="I29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29" t="str">
+        <f>"INSERT INTO PossessionsEquipements VALUES(" &amp; Tableau8[[#This Row],[IdPossessionEquipement]] &amp; "," &amp; Tableau8[[#This Row],[Chambre]] &amp;"," &amp; Tableau8[[#This Row],[Equipement]] &amp;");"</f>
+        <v>INSERT INTO PossessionsEquipements VALUES(5,5,3);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
       <c r="B32" t="s">
         <v>71</v>
       </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
       <c r="D32" t="s">
         <v>76</v>
       </c>
@@ -1730,14 +1950,21 @@
       <c r="G32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>72</v>
       </c>
+      <c r="C33" t="str">
+        <f>"INSERT INTO TypesPaiements VALUES(" &amp; Tableau9[[#This Row],[IdTypePaiement]] &amp; ",""" &amp; Tableau9[[#This Row],[LibelleTypePaiement]] &amp; """);"</f>
+        <v>INSERT INTO TypesPaiements VALUES(1,"Espèces");</v>
+      </c>
       <c r="D33">
         <v>1</v>
       </c>
@@ -1750,14 +1977,22 @@
       <c r="G33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f>"INSERT INTO Prestations VALUES(" &amp; Tableau10[[#This Row],[IdPrestation]] &amp; ",""" &amp; Tableau10[[#This Row],[LibellePrestation]] &amp; """,""" &amp; Tableau10[[#This Row],[DescriptionPrestation]] &amp; """," &amp; Tableau10[[#This Row],[PrixPrestation]] &amp; ");"</f>
+        <v>INSERT INTO Prestations VALUES(1,"Petit-déjeuner","Petit-déjeuner servi dans la salle de restauration",5);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>73</v>
       </c>
+      <c r="C34" t="str">
+        <f>"INSERT INTO TypesPaiements VALUES(" &amp; Tableau9[[#This Row],[IdTypePaiement]] &amp; ",""" &amp; Tableau9[[#This Row],[LibelleTypePaiement]] &amp; """);"</f>
+        <v>INSERT INTO TypesPaiements VALUES(2,"Carte bancaire");</v>
+      </c>
       <c r="D34">
         <v>2</v>
       </c>
@@ -1767,17 +2002,25 @@
       <c r="F34" t="s">
         <v>93</v>
       </c>
-      <c r="G34">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>138</v>
+      </c>
+      <c r="H34" t="str">
+        <f>"INSERT INTO Prestations VALUES(" &amp; Tableau10[[#This Row],[IdPrestation]] &amp; ",""" &amp; Tableau10[[#This Row],[LibellePrestation]] &amp; """,""" &amp; Tableau10[[#This Row],[DescriptionPrestation]] &amp; """," &amp; Tableau10[[#This Row],[PrixPrestation]] &amp; ");"</f>
+        <v>INSERT INTO Prestations VALUES(2,"Petit-déjeuner en chambre","Petit-déjeuner servi directement en chambre par un de nos employés",8.99);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
       <c r="B35" t="s">
         <v>74</v>
       </c>
+      <c r="C35" t="str">
+        <f>"INSERT INTO TypesPaiements VALUES(" &amp; Tableau9[[#This Row],[IdTypePaiement]] &amp; ",""" &amp; Tableau9[[#This Row],[LibelleTypePaiement]] &amp; """);"</f>
+        <v>INSERT INTO TypesPaiements VALUES(3,"Chèque");</v>
+      </c>
       <c r="D35">
         <v>3</v>
       </c>
@@ -1790,14 +2033,22 @@
       <c r="G35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <f>"INSERT INTO Prestations VALUES(" &amp; Tableau10[[#This Row],[IdPrestation]] &amp; ",""" &amp; Tableau10[[#This Row],[LibellePrestation]] &amp; """,""" &amp; Tableau10[[#This Row],[DescriptionPrestation]] &amp; """," &amp; Tableau10[[#This Row],[PrixPrestation]] &amp; ");"</f>
+        <v>INSERT INTO Prestations VALUES(3,"Réveil","Réveil par un employé de l'hôtel à une heure convenue",0);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>75</v>
       </c>
+      <c r="C36" t="str">
+        <f>"INSERT INTO TypesPaiements VALUES(" &amp; Tableau9[[#This Row],[IdTypePaiement]] &amp; ",""" &amp; Tableau9[[#This Row],[LibelleTypePaiement]] &amp; """);"</f>
+        <v>INSERT INTO TypesPaiements VALUES(4,"Chèque vacances");</v>
+      </c>
       <c r="D36">
         <v>4</v>
       </c>
@@ -1810,8 +2061,12 @@
       <c r="G36">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <f>"INSERT INTO Prestations VALUES(" &amp; Tableau10[[#This Row],[IdPrestation]] &amp; ",""" &amp; Tableau10[[#This Row],[LibellePrestation]] &amp; """,""" &amp; Tableau10[[#This Row],[DescriptionPrestation]] &amp; """," &amp; Tableau10[[#This Row],[PrixPrestation]] &amp; ");"</f>
+        <v>INSERT INTO Prestations VALUES(4,"Massage","Massage de détente réalisé par notre masseur partenaire",45);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>5</v>
       </c>
@@ -1821,11 +2076,15 @@
       <c r="F37" t="s">
         <v>88</v>
       </c>
-      <c r="G37">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>139</v>
+      </c>
+      <c r="H37" t="str">
+        <f>"INSERT INTO Prestations VALUES(" &amp; Tableau10[[#This Row],[IdPrestation]] &amp; ",""" &amp; Tableau10[[#This Row],[LibellePrestation]] &amp; """,""" &amp; Tableau10[[#This Row],[DescriptionPrestation]] &amp; """," &amp; Tableau10[[#This Row],[PrixPrestation]] &amp; ");"</f>
+        <v>INSERT INTO Prestations VALUES(5,"Lit d'appoint","Ajout d'un lit d'appoint dans une chambre",14.99);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1835,8 +2094,11 @@
       <c r="C40" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1846,8 +2108,12 @@
       <c r="C41" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D41" t="str">
+        <f>"INSERT INTO Fidelites VALUES(" &amp; Tableau11[[#This Row],[IdFidelite]] &amp; ",""" &amp; Tableau11[[#This Row],[LibelleFidelite]] &amp; """,""" &amp; Tableau11[[#This Row],[DescriptionFidelite]] &amp; """);"</f>
+        <v>INSERT INTO Fidelites VALUES(1,"Bronze","Réduction de 5% sur les chambres de type Standard");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1857,8 +2123,12 @@
       <c r="C42" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D42" t="str">
+        <f>"INSERT INTO Fidelites VALUES(" &amp; Tableau11[[#This Row],[IdFidelite]] &amp; ",""" &amp; Tableau11[[#This Row],[LibelleFidelite]] &amp; """,""" &amp; Tableau11[[#This Row],[DescriptionFidelite]] &amp; """);"</f>
+        <v>INSERT INTO Fidelites VALUES(2,"Argent","Réduction de 10% sur les chambres de type Standard et de 5% sur les chambres Deluxe");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -1868,8 +2138,12 @@
       <c r="C43" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" t="str">
+        <f>"INSERT INTO Fidelites VALUES(" &amp; Tableau11[[#This Row],[IdFidelite]] &amp; ",""" &amp; Tableau11[[#This Row],[LibelleFidelite]] &amp; """,""" &amp; Tableau11[[#This Row],[DescriptionFidelite]] &amp; """);"</f>
+        <v>INSERT INTO Fidelites VALUES(3,"Or","Réduction de 15% sur les chambres Standard et Deluxe, 5% sur les suites, consommation du mini-bar offerte le premier jour, petit-déjeuner en chambre à prix réduit");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1879,8 +2153,12 @@
       <c r="C44" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D44" t="str">
+        <f>"INSERT INTO Fidelites VALUES(" &amp; Tableau11[[#This Row],[IdFidelite]] &amp; ",""" &amp; Tableau11[[#This Row],[LibelleFidelite]] &amp; """,""" &amp; Tableau11[[#This Row],[DescriptionFidelite]] &amp; """);"</f>
+        <v>INSERT INTO Fidelites VALUES(4,"Platine","Réduction de 20% sur le séjour, 50% de réduction sur le premier massage");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -1894,7 +2172,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Changement cahier des charges + Mise à jour donnees.sql
</commit_message>
<xml_diff>
--- a/Base de données/Jeu de données.xlsx
+++ b/Base de données/Jeu de données.xlsx
@@ -1060,8 +1060,8 @@
     <tableColumn id="1" name="IdHistorique"/>
     <tableColumn id="2" name="Chambre"/>
     <tableColumn id="3" name="Reservations"/>
-    <tableColumn id="4" name="Colonne1" dataDxfId="1">
-      <calculatedColumnFormula>"INSERT INTO HistoriquesChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</calculatedColumnFormula>
+    <tableColumn id="4" name="Colonne1" dataDxfId="0">
+      <calculatedColumnFormula>"INSERT INTO HistoriqueChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1093,7 +1093,7 @@
     <tableColumn id="1" name="IdTypeChambre"/>
     <tableColumn id="2" name="LibelleTypeChambre"/>
     <tableColumn id="3" name="PrixChambre"/>
-    <tableColumn id="4" name="Colonne1" dataDxfId="0">
+    <tableColumn id="4" name="Colonne1" dataDxfId="1">
       <calculatedColumnFormula>"INSERT INTO TypesChambres VALUES(" &amp; Tableau3[[#This Row],[IdTypeChambre]] &amp; ",""" &amp; Tableau3[[#This Row],[LibelleTypeChambre]] &amp; """," &amp; Tableau3[[#This Row],[PrixChambre]] &amp; ");"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1456,7 +1456,7 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D92" sqref="D91:D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,8 +3129,8 @@
         <v>1</v>
       </c>
       <c r="D91" t="str">
-        <f>"INSERT INTO HistoriquesChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
-        <v>INSERT INTO HistoriquesChambres VALUES(1,3,1);</v>
+        <f>"INSERT INTO HistoriqueChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
+        <v>INSERT INTO HistoriqueChambres VALUES(1,3,1);</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3144,8 +3144,8 @@
         <v>2</v>
       </c>
       <c r="D92" t="str">
-        <f>"INSERT INTO HistoriquesChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
-        <v>INSERT INTO HistoriquesChambres VALUES(2,3,2);</v>
+        <f>"INSERT INTO HistoriqueChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
+        <v>INSERT INTO HistoriqueChambres VALUES(2,3,2);</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3159,8 +3159,8 @@
         <v>2</v>
       </c>
       <c r="D93" t="str">
-        <f>"INSERT INTO HistoriquesChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
-        <v>INSERT INTO HistoriquesChambres VALUES(3,4,2);</v>
+        <f>"INSERT INTO HistoriqueChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
+        <v>INSERT INTO HistoriqueChambres VALUES(3,4,2);</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3174,8 +3174,8 @@
         <v>3</v>
       </c>
       <c r="D94" t="str">
-        <f>"INSERT INTO HistoriquesChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
-        <v>INSERT INTO HistoriquesChambres VALUES(4,2,3);</v>
+        <f>"INSERT INTO HistoriqueChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
+        <v>INSERT INTO HistoriqueChambres VALUES(4,2,3);</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3189,8 +3189,8 @@
         <v>4</v>
       </c>
       <c r="D95" t="str">
-        <f>"INSERT INTO HistoriquesChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
-        <v>INSERT INTO HistoriquesChambres VALUES(5,5,4);</v>
+        <f>"INSERT INTO HistoriqueChambres VALUES(" &amp; Tableau19[[#This Row],[IdHistorique]] &amp; "," &amp; Tableau19[[#This Row],[Chambre]] &amp; "," &amp; Tableau19[[#This Row],[Reservations]] &amp; ");"</f>
+        <v>INSERT INTO HistoriqueChambres VALUES(5,5,4);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>